<commit_message>
update staff_form and projectcreate Excel files
</commit_message>
<xml_diff>
--- a/public/UploadExample/projectcreate.xlsx
+++ b/public/UploadExample/projectcreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5041E445-FC4C-49A6-B739-F3FAA60D2E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9453B54-D07A-47E2-8358-258D88FF6E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>แบบ Form สร้าง Project สำหรับนักศึกษา</t>
   </si>
@@ -44,12 +44,6 @@
     <t>เป็นแพลตฟอร์มที่พัฒนาขึ้นเพื่อรวบรวมและจัดเก็บข้อมูลโปรเจกต์จบของนักศึกษาวิศวกรรมศาสตร์ มหาวิทยาลัยเชียงใหม่ โดยมีเป้าหมายเพื่อเป็นแหล่งข้อมูลกลางที่ช่วยให้การเข้าถึงโปรเจกต์เก่า ๆ เป็นไปอย่างสะดวกและเป็นระบบ นักศึกษาสามารถค้นหาและดูรายละเอียดโปรเจกต์จบจากรุ่นพี่เพื่อใช้เป็นแรงบันดาลใจหรือแนวทางในการพัฒนาผลงานต่อไป</t>
   </si>
   <si>
-    <t>แพลตฟอร์มสำหรับจัดเก็บข้อมูลโปรเจกต์จบของวิศวกรรมศาสตร์ มหาวิทยาลัยเชียงใหม่</t>
-  </si>
-  <si>
-    <t>Project Box: A Platform for Archiving Senior Projects at CMU Engineering</t>
-  </si>
-  <si>
     <t>อาจารย์ที่ปรึกษา</t>
   </si>
   <si>
@@ -71,76 +65,121 @@
     <t>Staff Role</t>
   </si>
   <si>
-    <t>อลิซ เทย์เลอร์</t>
-  </si>
-  <si>
-    <t>บ็อบ วิลเลียมส์</t>
-  </si>
-  <si>
-    <t>กรรมการภายนอก</t>
-  </si>
-  <si>
     <t>ชื่อ - นามสกุล</t>
   </si>
   <si>
     <t>COURSE NO :</t>
   </si>
   <si>
-    <t xml:space="preserve">จักรภพ </t>
-  </si>
-  <si>
-    <t>สร้อยวิชา</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ณัฏฐ์ </t>
-  </si>
-  <si>
-    <t>อุจะรัตน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ปิยพัชร </t>
-  </si>
-  <si>
-    <t>ขาวแสง</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ณฐพงศ์ </t>
-  </si>
-  <si>
-    <t>พงศาวลีศรี</t>
-  </si>
-  <si>
-    <t xml:space="preserve">พิชยุทธ </t>
-  </si>
-  <si>
-    <t>หันชัยเนาว์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ฐิดายุ </t>
-  </si>
-  <si>
-    <t>พึ่งธรรม</t>
-  </si>
-  <si>
     <t>SECLAB</t>
   </si>
   <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>น้องโน่</t>
-  </si>
-  <si>
-    <t>เองจ้า</t>
+    <t>Web application to find available seats in the Chiang Mai University Library</t>
+  </si>
+  <si>
+    <t>เว็บแอปพลิเคชันสำหรับการค้นหาตำแหน่งที่นั่งที่ยังว่างอยู่ภายในสำนักหอสมุดมหาวิทยาลัยเชียงใหม่</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>โครงงานนี้เป็นการพัฒนาเว็บแอปพลิเคชันสำหรับการค้นหาตำแหน่งที่นั่งที่ยังว่างอยู่ภายในสำนักหอสมุดมหาวิทยาลัยเชียงใหม่ เนื่องจากมีนักศึกษาเข้าใช้หอสมุดจำนวนมากโดยเฉพาะอย่างยิ่งในช่วงสอบ หากใช้งานเว็บแอปพลิเคชันนี้จะทำให้สามารถรู้ตำแหน่งที่นั่งที่ยังว่างอยู่ล่วงหน้าก่อนเข้าใช้หอสมุดได้ และไม่ต้องเสียเวลาในการเดินวนหาที่นั่งในแต่ละชั้น เพราะในเว็บแอปพลิเคชันนี้จะแสดงตำแหน่งที่นั่งที่ยังว่างอยู่ในแต่ละชั้นของหอสมุด จำนวนผู้ใช้งาน และจำนวนที่นั่งที่ยังว่างอยู่จากจำนวนที่นั่งทั้งหมดอีกด้วย โดยจะมีการใช้ Machine Learning ทำ Camera Object Detection ในการนับจำนวนคนและตรวจสอบที่นั่งที่ยังว่างอยู่จาก ESP32-CAM with OV2640 ที่จะทําการติดตั้งไว้ แล้วจึงส่งข้อมูลที่ได้มาที่เว็บแอปพลิชันเพื่อแสดงผลให้แก่ผู้ใช้งานเว็บแอปพลิชันนี้</t>
+  </si>
+  <si>
+    <t>ชวัลลักษณ์</t>
+  </si>
+  <si>
+    <t xml:space="preserve">แก้วมูล </t>
+  </si>
+  <si>
+    <t>อานันท์ สีห์พิทักษ์เกียรติ</t>
+  </si>
+  <si>
+    <t>กรรมการ</t>
+  </si>
+  <si>
+    <t>โดม โพธิกานนท์</t>
+  </si>
+  <si>
+    <t>ธนดล</t>
+  </si>
+  <si>
+    <t>ตระกูลขยัน</t>
+  </si>
+  <si>
+    <t>ลัชนา ระมิงค์วงศ์</t>
+  </si>
+  <si>
+    <t>IoT for Smart Classroom</t>
+  </si>
+  <si>
+    <t>ไอโอทีสำหรับห้องเรียนฉัจฉริยะ</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>ปุริวง</t>
+  </si>
+  <si>
+    <t>เลิศนันทพร</t>
+  </si>
+  <si>
+    <t>ชินวัตร อิศราดิสัยกุล</t>
+  </si>
+  <si>
+    <t>SDN Switch Management Application</t>
+  </si>
+  <si>
+    <t>แอปพลิเคชันจัดการเอสดีเอ็นสวิตช์</t>
+  </si>
+  <si>
+    <t>ปัจจุบันการใช้งาน SDN จำเป็นต้องมี Controller, SDN switch  และ Application ควบคุม โดยใช้ Application ผ่าน API ของ Controller จากนั้น Controller ไปสั่งควบคุม SND switch ที่จำเป็นต้องใช้ผู้เชี่ยวชาญด้านเครือข่ายที่สามารถประยุกต์ใช้งาน SDN และใช้ API ซึ่งโดยทั่วไปต้องใช้ความชำนาญสูง โดยถูกพิจารณาว่าซับซ้อนเกินไปสำหรับบุคคลทั่วไปและผู้ดูแลระบบที่ไม่ชำนาญ ดังนั้นโครงงานนี้จึงนำเสนอการพัฒนา application ด้วย Ansible ที่รองรับการใช้งาน API ของ Controller และสามารถตั้งค่าบน SDN switch ให้สามารถหา shortest path ระหว่างต้นทางกับปลายทางและกำหนดเส้นทางได้เองโดยที่ไม่ต้องอาศัยที่อยู่ปลายทางเพียงอย่างเดียวเช่น การพิจาราณาจากที่อยู่ต้นทาง เพื่อบุคคลที่ไม่ชำนาญการใช้ SND และ  API โดย applicationในโครงงานนี้พัฒนามาเพื่อใช้งานกับ Ryu Controller และใช้งานคู่กับโปรแกรมจำลอง  SDN switch ที่เรียกว่า Mininet  โดยผู้ใช้สามารถป้อนข้อมูลที่จำเป็น เช่น IP address  ผ่านทาง Graphic User Interface (GUI) จากนั้น Application  จะส่งการตั้งค่าไปยัง Controler ผ่าน API ของ Controller แล้ว Controller ไปตั้งค่าให้ SDN switchโดยอัตโนมัติ เพื่อความสะดวกรวดเร็วในการทำงานและง่ายต่อการจัดการเส้นทาง</t>
+  </si>
+  <si>
+    <t>811</t>
+  </si>
+  <si>
+    <t>ธนกฤต</t>
+  </si>
+  <si>
+    <t xml:space="preserve">โยกาส </t>
+  </si>
+  <si>
+    <t>ยุทธพงษ์ สมจิต</t>
+  </si>
+  <si>
+    <t>ณัฐนันท์ พรหมสุข</t>
+  </si>
+  <si>
+    <t>Okami's Quest</t>
+  </si>
+  <si>
+    <t>โอคามิ เควส</t>
+  </si>
+  <si>
+    <t>เกมแนวaction-3Dมุมมองแบบtop-view ผสมกับแนวsoul-like โดยผู้เล่นจะรับบทเป็นซามูไรชื่อว่า"โอคามิ(大神)" ที่ต้องเดินทางไปสังหารโชกุนของฝ่ายศัตรูโดยต้องฝ่าอุปสรรค์มากมายด้วยตัวคนเดียว ตามภารกิจที่ได้รับจากโชกุนฝั่งของตน โดยเนื้อเรื่อง ,ฉาก และsettingของเกมจะดําเนินอยู่ในยุคเซ็นโงคุของญี่ปุ่น
+ชื่อ โอคามิ มาจาก 大神 ที่แปลว่าพระเจ้าผู้ยิ่งใหญ่ ซึ่งเกิดจากตัวเอกของเรานั้นฆ่าไม่ตาย(ซึ่งเป็นคอนเซ็ปของเกมแนวsoul-like) และยังพ้องเสียงกับ ookami ที่แปลว่าหมาป่าอีกด้วย
+โดยตัวเกมจะเป็นเกมaction-platforming ที่ตัวเอกจะต้องสู้ศัตรูยากๆและแก้ปริศนาเพื่อผ่านด่านไปเรื่อยๆจนได้พบกับบอส โดยระหว่างทางผู้เล่นจะเจอกับจุดcheckpointที่สามารถนําค่าประสบการณ์ที่ได้รับจากการฆ่าศัตรูมาเพื่ออัปเกรดstatsได้(เช่น พลังโจมตี พลังชีวิต มานา สกิลต่างๆ) แต่หากผู้เล่นตายก่อนมาถึงcheckpoint ค่าประสบการณ์ทั้งหมดที่ยังไม่ได้ใช้จะตกอยู่ตรงจุดที่ผู้เล่นตาย ซึ่งผู้เล่นสามารถมาเก็บค่าประสบการณ์ที่ตกอยู่ได้ แต่หากผู้เล่นตายอีกรอบก่อนมาเก็บค่าประสบการณ์ ค่าประสบการณ์ที่ตกอยู่จะหายไปทั้งหมด
+ผู้พัฒนาตั้งใจจะให้ความสนุกของเกมอยู่ที่ศัตรูที่จะมีหลากหลายรูปแบบ และต้องใช้วิธีรับมือที่เหมาะสมแตกต่างกัน รวมทั้งความยากของเกมที่ไม่มากไม่น้อยจนเกินไปเพื่อให้ผู้เล่นสามารถสนุกกับเกมได้เป็นเวลานาน นอกจากนี้ก็หวังว่าpuzzleต่างๆในเกมจะช่วงให้ผู้เล่นได้ฝึกไหวพริบในการแก้ไขปัญหาอีกด้วย โดยกลุ่มผู้ใช้ของเกมนี้นั้นคือทุกเพศทุกวัยที่อยากท้าทายตัวเองและผ่อนคลายตัวเองด้วยการเล่นเกม
+อ้างอิง:
+เกมแนวsoulike คืออะไร?
+https://www.gamingdose.com/feature/souls-like-%E0%B8%84%E0%B8%B7%E0%B8%AD%E0%B8%AD%E0%B8%B0%E0%B9%84%E0%B8%A3-%E0%B8%A2%E0%B8%B2%E0%B8%81%E0%B9%81%E0%B8%84%E0%B9%88%E0%B9%84%E0%B8%AB%E0%B8%99%E0%B8%96%E0%B8%B6%E0%B8%87%E0%B8%96/</t>
+  </si>
+  <si>
+    <t>ณรรฐชนน</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ทองอนันต์ </t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>ปฏิเวธ วุฒิสารวัฒนา</t>
+  </si>
+  <si>
+    <t>กานต์ ปทานุคม</t>
   </si>
 </sst>
 </file>
@@ -183,7 +222,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +251,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -277,7 +322,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -288,6 +333,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,11 +351,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -588,91 +642,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="23.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="23.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="35" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="7"/>
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9"/>
       <c r="C2" s="2">
         <v>261492</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="1">
-        <v>640610622</v>
+        <v>620610783</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>16</v>
@@ -681,122 +735,186 @@
         <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="D5" s="8" t="s">
-        <v>30</v>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="1">
-        <v>640610632</v>
+        <v>620610792</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="D6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1">
-        <v>640610651</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="10" customFormat="1">
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>29</v>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E8" s="1">
         <v>640610630</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="D9" s="8" t="s">
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="10" customFormat="1">
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1">
-        <v>640610653</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="D10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1">
-        <v>640610627</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="D11" s="8" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="1">
-        <v>640610999</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="E12" s="1">
+        <v>620612150</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="H13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="H14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="10" customFormat="1">
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.399999999999999" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1">
+        <v>620610785</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9">
+      <c r="H17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9">
+      <c r="H18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" s="10" customFormat="1">
+      <c r="D19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Improve search page UI with responsive search mode selection
</commit_message>
<xml_diff>
--- a/public/UploadExample/projectcreate.xlsx
+++ b/public/UploadExample/projectcreate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9453B54-D07A-47E2-8358-258D88FF6E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9826F8-C262-4969-900D-7F1E480E76B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>แบบ Form สร้าง Project สำหรับนักศึกษา</t>
   </si>
@@ -180,6 +181,12 @@
   </si>
   <si>
     <t>กานต์ ปทานุคม</t>
+  </si>
+  <si>
+    <t>กรรมการภายนอก</t>
+  </si>
+  <si>
+    <t>อาจารย์ที่ปรึกษาร่วม</t>
   </si>
 </sst>
 </file>
@@ -339,18 +346,6 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,6 +354,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -644,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="23.4"/>
@@ -664,23 +671,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="2">
         <v>261492</v>
       </c>
@@ -701,10 +708,10 @@
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
@@ -769,8 +776,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="10" customFormat="1">
-      <c r="D7" s="11"/>
+    <row r="7" spans="1:9" s="6" customFormat="1">
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
@@ -817,8 +824,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="10" customFormat="1">
-      <c r="D11" s="11"/>
+    <row r="11" spans="1:9" s="6" customFormat="1">
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
@@ -865,8 +872,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="10" customFormat="1">
-      <c r="D15" s="11"/>
+    <row r="15" spans="1:9" s="6" customFormat="1">
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="20.399999999999999" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -875,7 +882,7 @@
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -913,8 +920,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="4:9" s="10" customFormat="1">
-      <c r="D19" s="11"/>
+    <row r="19" spans="4:9" s="6" customFormat="1">
+      <c r="D19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -923,5 +930,56 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54BEFC8A-F0C4-441F-BBD5-9670BB4B75FB}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I1:I1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA34EC8-9CB5-4C9D-ACFD-1AD737BE4688}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor keyword management: update API endpoints, add editKeyword function, and adjust environment variables
</commit_message>
<xml_diff>
--- a/public/UploadExample/projectcreate.xlsx
+++ b/public/UploadExample/projectcreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89CA70B-84D8-4ED3-B0D6-AA49E6192012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF27AB1-251C-41E1-82D6-4A2EF3FDA8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,6 +1421,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1431,9 +1434,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1743,7 +1743,7 @@
   <dimension ref="A1:K163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1756,27 +1756,27 @@
     <col min="8" max="8" width="39.109375" style="8" customWidth="1"/>
     <col min="9" max="9" width="8.88671875" style="8"/>
     <col min="10" max="10" width="30.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="1">
         <v>261492</v>
       </c>
@@ -1803,10 +1803,10 @@
       <c r="E3" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1848,7 +1848,7 @@
       <c r="J4" t="s">
         <v>398</v>
       </c>
-      <c r="K4" s="14" t="b">
+      <c r="K4" s="10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1908,7 +1908,7 @@
       <c r="I8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -1968,7 +1968,7 @@
       <c r="I12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="10" t="s">
         <v>396</v>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       <c r="I16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       <c r="I20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
       <c r="I24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       <c r="I28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2259,7 +2259,7 @@
       <c r="I32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       <c r="I36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K36" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2376,7 +2376,7 @@
       <c r="I40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K40" s="14" t="s">
+      <c r="K40" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2448,7 +2448,7 @@
       <c r="I44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="K44" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2508,7 +2508,7 @@
       <c r="I48" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K48" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2580,7 +2580,7 @@
       <c r="I52" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K52" s="14" t="s">
+      <c r="K52" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2640,7 +2640,7 @@
       <c r="I56" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K56" s="14" t="s">
+      <c r="K56" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2700,7 +2700,7 @@
       <c r="I60" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K60" s="14" t="s">
+      <c r="K60" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
       <c r="I64" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K64" s="14" t="s">
+      <c r="K64" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       <c r="I68" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K68" s="14" t="s">
+      <c r="K68" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2865,7 +2865,7 @@
       <c r="I72" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K72" s="14" t="s">
+      <c r="K72" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2922,7 +2922,7 @@
       <c r="I76" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K76" s="14" t="s">
+      <c r="K76" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
       <c r="I80" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K80" s="14" t="s">
+      <c r="K80" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
       <c r="I84" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K84" s="14" t="s">
+      <c r="K84" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3090,7 +3090,7 @@
       <c r="I88" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K88" s="14" t="s">
+      <c r="K88" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3138,7 +3138,7 @@
       <c r="I92" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K92" s="14" t="s">
+      <c r="K92" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3210,7 +3210,7 @@
       <c r="I96" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K96" s="14" t="s">
+      <c r="K96" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3270,7 +3270,7 @@
       <c r="I100" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K100" s="14" t="s">
+      <c r="K100" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3330,7 +3330,7 @@
       <c r="I104" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K104" s="14" t="s">
+      <c r="K104" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3390,7 +3390,7 @@
       <c r="I108" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K108" s="14" t="s">
+      <c r="K108" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3450,7 +3450,7 @@
       <c r="I112" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K112" s="14" t="s">
+      <c r="K112" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3510,7 +3510,7 @@
       <c r="I116" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K116" s="14" t="s">
+      <c r="K116" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3570,7 +3570,7 @@
       <c r="I120" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K120" s="14" t="s">
+      <c r="K120" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3630,7 +3630,7 @@
       <c r="I124" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K124" s="14" t="s">
+      <c r="K124" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
       <c r="I128" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K128" s="14" t="s">
+      <c r="K128" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3762,7 +3762,7 @@
       <c r="I132" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K132" s="14" t="s">
+      <c r="K132" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3810,7 +3810,7 @@
       <c r="I136" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K136" s="14" t="s">
+      <c r="K136" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3870,7 +3870,7 @@
       <c r="I140" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K140" s="14" t="s">
+      <c r="K140" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3918,7 +3918,7 @@
       <c r="I144" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K144" s="14" t="s">
+      <c r="K144" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3978,7 +3978,7 @@
       <c r="I148" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K148" s="14" t="s">
+      <c r="K148" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -4038,7 +4038,7 @@
       <c r="I152" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K152" s="14" t="s">
+      <c r="K152" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -4086,7 +4086,7 @@
       <c r="I156" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K156" s="14" t="s">
+      <c r="K156" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -4142,7 +4142,7 @@
       <c r="I161" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K161" s="14" t="s">
+      <c r="K161" s="10" t="s">
         <v>397</v>
       </c>
     </row>

</xml_diff>